<commit_message>
fixed story_display closing q19 too quickly
</commit_message>
<xml_diff>
--- a/editable/text_files/Orders/PAR01_RUN01.xlsx
+++ b/editable/text_files/Orders/PAR01_RUN01.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evade\Documents\GitHub\Zoom_ToM\editable\Orders\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\evade\Documents\GitHub\Zoom_ToM\editable\Orders\Orders\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8776F81-C242-4491-87A6-2F4D36894612}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49AE57AB-6B0B-48B3-A2B7-A250D5B74E85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6612" yWindow="0" windowWidth="16428" windowHeight="12360" xr2:uid="{C5687CB1-4EE8-4A5B-BACE-F200205D7D06}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{FC6C8707-799B-4B80-8D55-E991A8407F1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
     <t>Question</t>
   </si>
   <si>
-    <t>RunType</t>
+    <t>ConditionType</t>
   </si>
 </sst>
 </file>
@@ -392,7 +392,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E82E2DDB-476F-41D8-B03D-1EE8DB8FC8DA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4B58521-7983-4D32-8C1E-5EE9228DA121}">
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -417,10 +417,10 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -428,10 +428,10 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -439,10 +439,10 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -450,10 +450,10 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -461,10 +461,10 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -472,10 +472,10 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -483,10 +483,10 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -494,10 +494,10 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -505,10 +505,10 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -516,10 +516,10 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -530,7 +530,7 @@
         <v>9</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -538,10 +538,10 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -549,10 +549,10 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="C14">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -560,10 +560,10 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -571,10 +571,10 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -582,10 +582,10 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -593,10 +593,10 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -604,10 +604,10 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -615,10 +615,10 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>